<commit_message>
El endpoint Para crear informes funciona
</commit_message>
<xml_diff>
--- a/backend/api/src/templates/report.xlsx
+++ b/backend/api/src/templates/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toloz\Documents\VSC\clashOfClansApi\backend\api\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B8E9D4-451E-45CF-9813-572E90B9C9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1081B49D-EC3B-4F66-B94E-59BAC1D7390C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7E4F33C7-B692-4A7F-93A3-CBF16A756215}"/>
   </bookViews>
@@ -107,14 +107,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
+      <sz val="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -164,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -289,11 +289,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -322,109 +357,112 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -764,209 +802,205 @@
   <dimension ref="A1:S67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" customWidth="1"/>
-    <col min="7" max="8" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" customWidth="1"/>
+    <col min="10" max="15" width="6.5703125" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="13"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="20"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="15"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="21"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="22" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="22" t="s">
+      <c r="G4" s="37"/>
+      <c r="H4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="28" t="s">
+      <c r="I4" s="37"/>
+      <c r="J4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="28" t="s">
+      <c r="K4" s="32"/>
+      <c r="L4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="29"/>
-      <c r="N4" s="28" t="s">
+      <c r="M4" s="32"/>
+      <c r="N4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="O4" s="29"/>
-      <c r="P4" s="34" t="s">
+      <c r="O4" s="32"/>
+      <c r="P4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="35"/>
+      <c r="Q4" s="28"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="24" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="24" t="s">
+      <c r="E5" s="39"/>
+      <c r="F5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="24" t="s">
+      <c r="G5" s="39"/>
+      <c r="H5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="25"/>
-      <c r="J5" s="30" t="s">
+      <c r="I5" s="39"/>
+      <c r="J5" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="30" t="s">
+      <c r="K5" s="42"/>
+      <c r="L5" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="31"/>
-      <c r="N5" s="30" t="s">
+      <c r="M5" s="42"/>
+      <c r="N5" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="31"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="37"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="26" t="s">
+      <c r="O5" s="42"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="30"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="33" t="s">
+      <c r="K6" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="32" t="s">
+      <c r="L6" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="32" t="s">
+      <c r="N6" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="33" t="s">
+      <c r="O6" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="38" t="s">
+      <c r="P6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Q6" s="39" t="s">
+      <c r="Q6" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="3"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="49"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="45"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
       <c r="F8" s="5"/>
@@ -986,9 +1020,9 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="45"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
@@ -1005,9 +1039,9 @@
       <c r="Q9" s="6"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="45"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
@@ -1024,9 +1058,9 @@
       <c r="Q10" s="6"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="45"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
@@ -1043,28 +1077,28 @@
       <c r="Q11" s="6"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="6"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="49"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="45"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
@@ -1081,9 +1115,9 @@
       <c r="Q13" s="6"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="45"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="5"/>
@@ -1100,9 +1134,9 @@
       <c r="Q14" s="6"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="45"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
       <c r="F15" s="5"/>
@@ -1118,48 +1152,48 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="6"/>
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="9"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="6"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="3"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="45"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
       <c r="F18" s="5"/>
@@ -1176,9 +1210,9 @@
       <c r="Q18" s="6"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="45"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
       <c r="F19" s="5"/>
@@ -1195,9 +1229,9 @@
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="13"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="45"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
       <c r="F20" s="5"/>
@@ -1213,48 +1247,48 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="6"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="6"/>
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="9"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="6"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="3"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="45"/>
+      <c r="C23" s="16"/>
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
       <c r="F23" s="5"/>
@@ -1271,9 +1305,9 @@
       <c r="Q23" s="6"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="45"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
       <c r="F24" s="5"/>
@@ -1290,9 +1324,9 @@
       <c r="Q24" s="6"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="45"/>
+      <c r="C25" s="16"/>
       <c r="D25" s="5"/>
       <c r="E25" s="6"/>
       <c r="F25" s="5"/>
@@ -1308,48 +1342,48 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="6"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="6"/>
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="9"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="6"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="48"/>
+      <c r="O27" s="49"/>
+      <c r="P27" s="48"/>
+      <c r="Q27" s="49"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="45"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
       <c r="F28" s="5"/>
@@ -1366,9 +1400,9 @@
       <c r="Q28" s="6"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="45"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="5"/>
       <c r="E29" s="6"/>
       <c r="F29" s="5"/>
@@ -1385,9 +1419,9 @@
       <c r="Q29" s="6"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="45"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="5"/>
       <c r="E30" s="6"/>
       <c r="F30" s="5"/>
@@ -1404,9 +1438,9 @@
       <c r="Q30" s="6"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="45"/>
+      <c r="C31" s="16"/>
       <c r="D31" s="5"/>
       <c r="E31" s="6"/>
       <c r="F31" s="5"/>
@@ -1423,28 +1457,28 @@
       <c r="Q31" s="6"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="6"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="48"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="48"/>
+      <c r="Q32" s="49"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="45"/>
+      <c r="C33" s="16"/>
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
       <c r="F33" s="5"/>
@@ -1461,9 +1495,9 @@
       <c r="Q33" s="6"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="45"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
       <c r="F34" s="5"/>
@@ -1480,9 +1514,9 @@
       <c r="Q34" s="6"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="42"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="45"/>
+      <c r="C35" s="16"/>
       <c r="D35" s="5"/>
       <c r="E35" s="6"/>
       <c r="F35" s="5"/>
@@ -1498,48 +1532,48 @@
       <c r="P35" s="5"/>
       <c r="Q35" s="6"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="6"/>
+    <row r="36" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="9"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="42"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="6"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="3"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="4"/>
-      <c r="C38" s="45"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="5"/>
       <c r="E38" s="6"/>
       <c r="F38" s="5"/>
@@ -1556,9 +1590,9 @@
       <c r="Q38" s="6"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="4"/>
-      <c r="C39" s="45"/>
+      <c r="C39" s="16"/>
       <c r="D39" s="5"/>
       <c r="E39" s="6"/>
       <c r="F39" s="5"/>
@@ -1575,9 +1609,9 @@
       <c r="Q39" s="6"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
+      <c r="A40" s="13"/>
       <c r="B40" s="4"/>
-      <c r="C40" s="45"/>
+      <c r="C40" s="16"/>
       <c r="D40" s="5"/>
       <c r="E40" s="6"/>
       <c r="F40" s="5"/>
@@ -1593,48 +1627,48 @@
       <c r="P40" s="5"/>
       <c r="Q40" s="6"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="42"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="6"/>
+    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="14"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="9"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="6"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="3"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="42"/>
+      <c r="A43" s="13"/>
       <c r="B43" s="4"/>
-      <c r="C43" s="45"/>
+      <c r="C43" s="16"/>
       <c r="D43" s="5"/>
       <c r="E43" s="6"/>
       <c r="F43" s="5"/>
@@ -1651,9 +1685,9 @@
       <c r="Q43" s="6"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
+      <c r="A44" s="13"/>
       <c r="B44" s="4"/>
-      <c r="C44" s="45"/>
+      <c r="C44" s="16"/>
       <c r="D44" s="5"/>
       <c r="E44" s="6"/>
       <c r="F44" s="5"/>
@@ -1670,9 +1704,9 @@
       <c r="Q44" s="6"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="42"/>
+      <c r="A45" s="13"/>
       <c r="B45" s="4"/>
-      <c r="C45" s="45"/>
+      <c r="C45" s="16"/>
       <c r="D45" s="5"/>
       <c r="E45" s="6"/>
       <c r="F45" s="5"/>
@@ -1688,48 +1722,48 @@
       <c r="P45" s="5"/>
       <c r="Q45" s="6"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="42"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="6"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="6"/>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="6"/>
+    <row r="46" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="14"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="9"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="9"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="42"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="6"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="6"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="6"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="3"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="42"/>
+      <c r="A48" s="13"/>
       <c r="B48" s="4"/>
-      <c r="C48" s="45"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="5"/>
       <c r="E48" s="6"/>
       <c r="F48" s="5"/>
@@ -1746,9 +1780,9 @@
       <c r="Q48" s="6"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A49" s="42"/>
+      <c r="A49" s="13"/>
       <c r="B49" s="4"/>
-      <c r="C49" s="45"/>
+      <c r="C49" s="16"/>
       <c r="D49" s="5"/>
       <c r="E49" s="6"/>
       <c r="F49" s="5"/>
@@ -1765,9 +1799,9 @@
       <c r="Q49" s="6"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A50" s="42"/>
+      <c r="A50" s="13"/>
       <c r="B50" s="4"/>
-      <c r="C50" s="45"/>
+      <c r="C50" s="16"/>
       <c r="D50" s="5"/>
       <c r="E50" s="6"/>
       <c r="F50" s="5"/>
@@ -1783,48 +1817,48 @@
       <c r="P50" s="5"/>
       <c r="Q50" s="6"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51" s="42"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="6"/>
-      <c r="P51" s="5"/>
-      <c r="Q51" s="6"/>
+    <row r="51" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="14"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="9"/>
+      <c r="P51" s="8"/>
+      <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" s="42"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="6"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="6"/>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="6"/>
+      <c r="A52" s="12"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="3"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" s="42"/>
+      <c r="A53" s="13"/>
       <c r="B53" s="4"/>
-      <c r="C53" s="45"/>
+      <c r="C53" s="16"/>
       <c r="D53" s="5"/>
       <c r="E53" s="6"/>
       <c r="F53" s="5"/>
@@ -1841,9 +1875,9 @@
       <c r="Q53" s="6"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A54" s="42"/>
+      <c r="A54" s="13"/>
       <c r="B54" s="4"/>
-      <c r="C54" s="45"/>
+      <c r="C54" s="16"/>
       <c r="D54" s="5"/>
       <c r="E54" s="6"/>
       <c r="F54" s="5"/>
@@ -1860,9 +1894,9 @@
       <c r="Q54" s="6"/>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A55" s="42"/>
+      <c r="A55" s="13"/>
       <c r="B55" s="4"/>
-      <c r="C55" s="45"/>
+      <c r="C55" s="16"/>
       <c r="D55" s="5"/>
       <c r="E55" s="6"/>
       <c r="F55" s="5"/>
@@ -1878,29 +1912,29 @@
       <c r="P55" s="5"/>
       <c r="Q55" s="6"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A56" s="42"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="6"/>
-      <c r="N56" s="5"/>
-      <c r="O56" s="6"/>
-      <c r="P56" s="5"/>
-      <c r="Q56" s="6"/>
+    <row r="56" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="14"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="9"/>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A57" s="42"/>
+      <c r="A57" s="13"/>
       <c r="B57" s="4"/>
-      <c r="C57" s="45"/>
+      <c r="C57" s="16"/>
       <c r="D57" s="5"/>
       <c r="E57" s="6"/>
       <c r="F57" s="5"/>
@@ -1917,9 +1951,9 @@
       <c r="Q57" s="6"/>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A58" s="42"/>
+      <c r="A58" s="13"/>
       <c r="B58" s="4"/>
-      <c r="C58" s="45"/>
+      <c r="C58" s="16"/>
       <c r="D58" s="5"/>
       <c r="E58" s="6"/>
       <c r="F58" s="5"/>
@@ -1936,9 +1970,9 @@
       <c r="Q58" s="6"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A59" s="42"/>
+      <c r="A59" s="13"/>
       <c r="B59" s="4"/>
-      <c r="C59" s="45"/>
+      <c r="C59" s="16"/>
       <c r="D59" s="5"/>
       <c r="E59" s="6"/>
       <c r="F59" s="5"/>
@@ -1955,9 +1989,9 @@
       <c r="Q59" s="6"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A60" s="42"/>
+      <c r="A60" s="13"/>
       <c r="B60" s="4"/>
-      <c r="C60" s="45"/>
+      <c r="C60" s="16"/>
       <c r="D60" s="5"/>
       <c r="E60" s="6"/>
       <c r="F60" s="5"/>
@@ -1974,9 +2008,9 @@
       <c r="Q60" s="6"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A61" s="42"/>
+      <c r="A61" s="13"/>
       <c r="B61" s="4"/>
-      <c r="C61" s="45"/>
+      <c r="C61" s="16"/>
       <c r="D61" s="5"/>
       <c r="E61" s="6"/>
       <c r="F61" s="5"/>
@@ -1993,9 +2027,9 @@
       <c r="Q61" s="6"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A62" s="42"/>
+      <c r="A62" s="13"/>
       <c r="B62" s="4"/>
-      <c r="C62" s="45"/>
+      <c r="C62" s="16"/>
       <c r="D62" s="5"/>
       <c r="E62" s="6"/>
       <c r="F62" s="5"/>
@@ -2012,9 +2046,9 @@
       <c r="Q62" s="6"/>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A63" s="42"/>
+      <c r="A63" s="13"/>
       <c r="B63" s="4"/>
-      <c r="C63" s="45"/>
+      <c r="C63" s="16"/>
       <c r="D63" s="5"/>
       <c r="E63" s="6"/>
       <c r="F63" s="5"/>
@@ -2031,9 +2065,9 @@
       <c r="Q63" s="6"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A64" s="42"/>
+      <c r="A64" s="13"/>
       <c r="B64" s="4"/>
-      <c r="C64" s="45"/>
+      <c r="C64" s="16"/>
       <c r="D64" s="5"/>
       <c r="E64" s="6"/>
       <c r="F64" s="5"/>
@@ -2050,9 +2084,9 @@
       <c r="Q64" s="6"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A65" s="42"/>
+      <c r="A65" s="13"/>
       <c r="B65" s="4"/>
-      <c r="C65" s="45"/>
+      <c r="C65" s="16"/>
       <c r="D65" s="5"/>
       <c r="E65" s="6"/>
       <c r="F65" s="5"/>
@@ -2069,9 +2103,9 @@
       <c r="Q65" s="6"/>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A66" s="42"/>
+      <c r="A66" s="13"/>
       <c r="B66" s="4"/>
-      <c r="C66" s="45"/>
+      <c r="C66" s="16"/>
       <c r="D66" s="5"/>
       <c r="E66" s="6"/>
       <c r="F66" s="5"/>
@@ -2088,9 +2122,9 @@
       <c r="Q66" s="6"/>
     </row>
     <row r="67" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="43"/>
+      <c r="A67" s="14"/>
       <c r="B67" s="7"/>
-      <c r="C67" s="46"/>
+      <c r="C67" s="17"/>
       <c r="D67" s="8"/>
       <c r="E67" s="9"/>
       <c r="F67" s="8"/>
@@ -2108,6 +2142,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="N2:O3"/>
     <mergeCell ref="P2:Q3"/>
     <mergeCell ref="B2:M3"/>
@@ -2124,9 +2161,6 @@
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
arregle bugs y mejore otras cosas
</commit_message>
<xml_diff>
--- a/backend/api/src/templates/report.xlsx
+++ b/backend/api/src/templates/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toloz\Documents\VSC\clashOfClansApi\backend\api\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1081B49D-EC3B-4F66-B94E-59BAC1D7390C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25686BD-3292-4DBD-93D3-A641BA43E12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7E4F33C7-B692-4A7F-93A3-CBF16A756215}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E4F33C7-B692-4A7F-93A3-CBF16A756215}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
   <si>
     <t xml:space="preserve">Reporte del Clan </t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Fecha de unión</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Asaltos de Clan</t>
@@ -375,6 +372,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -402,25 +434,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -428,42 +461,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -802,202 +799,222 @@
   <dimension ref="A1:S67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" customWidth="1"/>
-    <col min="10" max="15" width="6.5703125" customWidth="1"/>
-    <col min="16" max="16" width="10" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" customWidth="1"/>
+    <col min="10" max="17" width="6.5546875" customWidth="1"/>
+    <col min="18" max="19" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="20"/>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="23"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="21"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="25" t="s">
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="33"/>
+    </row>
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="36"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="34"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="41"/>
+      <c r="F4" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="41"/>
+      <c r="H4" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="41"/>
+      <c r="J4" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="43"/>
+      <c r="L4" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="43"/>
+      <c r="N4" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="43"/>
+      <c r="P4" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="S4" s="45"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="37"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="28"/>
+      <c r="H5" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="J5" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="30"/>
+      <c r="L5" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="30"/>
+      <c r="N5" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="30"/>
+      <c r="P5" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="47"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="37"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="36" t="s">
+      <c r="E6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="36" t="s">
+      <c r="G6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="37"/>
-      <c r="J4" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="M4" s="32"/>
-      <c r="N4" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="O4" s="32"/>
-      <c r="P4" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q4" s="28"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="39"/>
-      <c r="J5" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="M5" s="42"/>
-      <c r="N5" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" s="42"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="30"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="43" t="s">
+      <c r="I6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="44" t="s">
+      <c r="J6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="M6" s="44" t="s">
+      <c r="L6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="O6" s="44" t="s">
+      <c r="N6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="O6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="P6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="S6" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="48"/>
-      <c r="Q7" s="49"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="26"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="13"/>
       <c r="B8" s="4"/>
       <c r="C8" s="16"/>
@@ -1015,11 +1032,10 @@
       <c r="O8" s="6"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="6"/>
-      <c r="S8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R8" s="5"/>
+      <c r="S8" s="6"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="13"/>
       <c r="B9" s="4"/>
       <c r="C9" s="16"/>
@@ -1037,8 +1053,10 @@
       <c r="O9" s="6"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="6"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R9" s="5"/>
+      <c r="S9" s="6"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="4"/>
       <c r="C10" s="16"/>
@@ -1056,8 +1074,10 @@
       <c r="O10" s="6"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="6"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R10" s="5"/>
+      <c r="S10" s="6"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="4"/>
       <c r="C11" s="16"/>
@@ -1075,27 +1095,31 @@
       <c r="O11" s="6"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="6"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="49"/>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="49"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R11" s="5"/>
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="26"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="4"/>
       <c r="C13" s="16"/>
@@ -1113,8 +1137,10 @@
       <c r="O13" s="6"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="6"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R13" s="5"/>
+      <c r="S13" s="6"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="4"/>
       <c r="C14" s="16"/>
@@ -1132,8 +1158,10 @@
       <c r="O14" s="6"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="6"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R14" s="5"/>
+      <c r="S14" s="6"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="4"/>
       <c r="C15" s="16"/>
@@ -1151,8 +1179,10 @@
       <c r="O15" s="6"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="6"/>
-    </row>
-    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R15" s="5"/>
+      <c r="S15" s="6"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14"/>
       <c r="B16" s="7"/>
       <c r="C16" s="17"/>
@@ -1170,8 +1200,10 @@
       <c r="O16" s="9"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="9"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="8"/>
+      <c r="S16" s="9"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="1"/>
       <c r="C17" s="15"/>
@@ -1189,8 +1221,10 @@
       <c r="O17" s="3"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="3"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="2"/>
+      <c r="S17" s="3"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="4"/>
       <c r="C18" s="16"/>
@@ -1208,8 +1242,10 @@
       <c r="O18" s="6"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="6"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="5"/>
+      <c r="S18" s="6"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="4"/>
       <c r="C19" s="16"/>
@@ -1227,8 +1263,10 @@
       <c r="O19" s="6"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="6"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" s="5"/>
+      <c r="S19" s="6"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="4"/>
       <c r="C20" s="16"/>
@@ -1246,8 +1284,10 @@
       <c r="O20" s="6"/>
       <c r="P20" s="5"/>
       <c r="Q20" s="6"/>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R20" s="5"/>
+      <c r="S20" s="6"/>
+    </row>
+    <row r="21" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14"/>
       <c r="B21" s="7"/>
       <c r="C21" s="17"/>
@@ -1265,8 +1305,10 @@
       <c r="O21" s="9"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="9"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21" s="8"/>
+      <c r="S21" s="9"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="1"/>
       <c r="C22" s="15"/>
@@ -1284,8 +1326,10 @@
       <c r="O22" s="3"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="3"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" s="2"/>
+      <c r="S22" s="3"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="4"/>
       <c r="C23" s="16"/>
@@ -1303,8 +1347,10 @@
       <c r="O23" s="6"/>
       <c r="P23" s="5"/>
       <c r="Q23" s="6"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23" s="5"/>
+      <c r="S23" s="6"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="4"/>
       <c r="C24" s="16"/>
@@ -1322,8 +1368,10 @@
       <c r="O24" s="6"/>
       <c r="P24" s="5"/>
       <c r="Q24" s="6"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24" s="5"/>
+      <c r="S24" s="6"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="4"/>
       <c r="C25" s="16"/>
@@ -1341,8 +1389,10 @@
       <c r="O25" s="6"/>
       <c r="P25" s="5"/>
       <c r="Q25" s="6"/>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R25" s="5"/>
+      <c r="S25" s="6"/>
+    </row>
+    <row r="26" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14"/>
       <c r="B26" s="7"/>
       <c r="C26" s="17"/>
@@ -1360,27 +1410,31 @@
       <c r="O26" s="9"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="9"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="45"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="48"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="48"/>
-      <c r="O27" s="49"/>
-      <c r="P27" s="48"/>
-      <c r="Q27" s="49"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26" s="8"/>
+      <c r="S26" s="9"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="22"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="26"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="4"/>
       <c r="C28" s="16"/>
@@ -1398,8 +1452,10 @@
       <c r="O28" s="6"/>
       <c r="P28" s="5"/>
       <c r="Q28" s="6"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28" s="5"/>
+      <c r="S28" s="6"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="4"/>
       <c r="C29" s="16"/>
@@ -1417,8 +1473,10 @@
       <c r="O29" s="6"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="6"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R29" s="5"/>
+      <c r="S29" s="6"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="4"/>
       <c r="C30" s="16"/>
@@ -1436,8 +1494,10 @@
       <c r="O30" s="6"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="6"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30" s="5"/>
+      <c r="S30" s="6"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="4"/>
       <c r="C31" s="16"/>
@@ -1455,27 +1515,31 @@
       <c r="O31" s="6"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="6"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="45"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="48"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="48"/>
-      <c r="Q32" s="49"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R31" s="5"/>
+      <c r="S31" s="6"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32" s="22"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="26"/>
+      <c r="R32" s="25"/>
+      <c r="S32" s="26"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="4"/>
       <c r="C33" s="16"/>
@@ -1493,8 +1557,10 @@
       <c r="O33" s="6"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="6"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R33" s="5"/>
+      <c r="S33" s="6"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
       <c r="B34" s="4"/>
       <c r="C34" s="16"/>
@@ -1512,8 +1578,10 @@
       <c r="O34" s="6"/>
       <c r="P34" s="5"/>
       <c r="Q34" s="6"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34" s="5"/>
+      <c r="S34" s="6"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="4"/>
       <c r="C35" s="16"/>
@@ -1531,8 +1599,10 @@
       <c r="O35" s="6"/>
       <c r="P35" s="5"/>
       <c r="Q35" s="6"/>
-    </row>
-    <row r="36" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R35" s="5"/>
+      <c r="S35" s="6"/>
+    </row>
+    <row r="36" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="14"/>
       <c r="B36" s="7"/>
       <c r="C36" s="17"/>
@@ -1550,8 +1620,10 @@
       <c r="O36" s="9"/>
       <c r="P36" s="8"/>
       <c r="Q36" s="9"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R36" s="8"/>
+      <c r="S36" s="9"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="12"/>
       <c r="B37" s="1"/>
       <c r="C37" s="15"/>
@@ -1569,8 +1641,10 @@
       <c r="O37" s="3"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="3"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R37" s="2"/>
+      <c r="S37" s="3"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="4"/>
       <c r="C38" s="16"/>
@@ -1588,8 +1662,10 @@
       <c r="O38" s="6"/>
       <c r="P38" s="5"/>
       <c r="Q38" s="6"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R38" s="5"/>
+      <c r="S38" s="6"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
       <c r="B39" s="4"/>
       <c r="C39" s="16"/>
@@ -1607,8 +1683,10 @@
       <c r="O39" s="6"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="6"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R39" s="5"/>
+      <c r="S39" s="6"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="4"/>
       <c r="C40" s="16"/>
@@ -1626,8 +1704,10 @@
       <c r="O40" s="6"/>
       <c r="P40" s="5"/>
       <c r="Q40" s="6"/>
-    </row>
-    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R40" s="5"/>
+      <c r="S40" s="6"/>
+    </row>
+    <row r="41" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="14"/>
       <c r="B41" s="7"/>
       <c r="C41" s="17"/>
@@ -1645,8 +1725,10 @@
       <c r="O41" s="9"/>
       <c r="P41" s="8"/>
       <c r="Q41" s="9"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R41" s="8"/>
+      <c r="S41" s="9"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="12"/>
       <c r="B42" s="1"/>
       <c r="C42" s="15"/>
@@ -1664,8 +1746,10 @@
       <c r="O42" s="3"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="3"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R42" s="2"/>
+      <c r="S42" s="3"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="13"/>
       <c r="B43" s="4"/>
       <c r="C43" s="16"/>
@@ -1683,8 +1767,10 @@
       <c r="O43" s="6"/>
       <c r="P43" s="5"/>
       <c r="Q43" s="6"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R43" s="5"/>
+      <c r="S43" s="6"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="4"/>
       <c r="C44" s="16"/>
@@ -1702,8 +1788,10 @@
       <c r="O44" s="6"/>
       <c r="P44" s="5"/>
       <c r="Q44" s="6"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R44" s="5"/>
+      <c r="S44" s="6"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="13"/>
       <c r="B45" s="4"/>
       <c r="C45" s="16"/>
@@ -1721,8 +1809,10 @@
       <c r="O45" s="6"/>
       <c r="P45" s="5"/>
       <c r="Q45" s="6"/>
-    </row>
-    <row r="46" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R45" s="5"/>
+      <c r="S45" s="6"/>
+    </row>
+    <row r="46" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="14"/>
       <c r="B46" s="7"/>
       <c r="C46" s="17"/>
@@ -1740,8 +1830,10 @@
       <c r="O46" s="9"/>
       <c r="P46" s="8"/>
       <c r="Q46" s="9"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R46" s="8"/>
+      <c r="S46" s="9"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="12"/>
       <c r="B47" s="1"/>
       <c r="C47" s="15"/>
@@ -1759,8 +1851,10 @@
       <c r="O47" s="3"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="3"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R47" s="2"/>
+      <c r="S47" s="3"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="13"/>
       <c r="B48" s="4"/>
       <c r="C48" s="16"/>
@@ -1778,8 +1872,10 @@
       <c r="O48" s="6"/>
       <c r="P48" s="5"/>
       <c r="Q48" s="6"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R48" s="5"/>
+      <c r="S48" s="6"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="13"/>
       <c r="B49" s="4"/>
       <c r="C49" s="16"/>
@@ -1797,8 +1893,10 @@
       <c r="O49" s="6"/>
       <c r="P49" s="5"/>
       <c r="Q49" s="6"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R49" s="5"/>
+      <c r="S49" s="6"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="13"/>
       <c r="B50" s="4"/>
       <c r="C50" s="16"/>
@@ -1816,8 +1914,10 @@
       <c r="O50" s="6"/>
       <c r="P50" s="5"/>
       <c r="Q50" s="6"/>
-    </row>
-    <row r="51" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R50" s="5"/>
+      <c r="S50" s="6"/>
+    </row>
+    <row r="51" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="14"/>
       <c r="B51" s="7"/>
       <c r="C51" s="17"/>
@@ -1835,8 +1935,10 @@
       <c r="O51" s="9"/>
       <c r="P51" s="8"/>
       <c r="Q51" s="9"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R51" s="8"/>
+      <c r="S51" s="9"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="12"/>
       <c r="B52" s="1"/>
       <c r="C52" s="15"/>
@@ -1854,8 +1956,10 @@
       <c r="O52" s="3"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="3"/>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R52" s="2"/>
+      <c r="S52" s="3"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="13"/>
       <c r="B53" s="4"/>
       <c r="C53" s="16"/>
@@ -1873,8 +1977,10 @@
       <c r="O53" s="6"/>
       <c r="P53" s="5"/>
       <c r="Q53" s="6"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R53" s="5"/>
+      <c r="S53" s="6"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="13"/>
       <c r="B54" s="4"/>
       <c r="C54" s="16"/>
@@ -1892,8 +1998,10 @@
       <c r="O54" s="6"/>
       <c r="P54" s="5"/>
       <c r="Q54" s="6"/>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R54" s="5"/>
+      <c r="S54" s="6"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="13"/>
       <c r="B55" s="4"/>
       <c r="C55" s="16"/>
@@ -1911,8 +2019,10 @@
       <c r="O55" s="6"/>
       <c r="P55" s="5"/>
       <c r="Q55" s="6"/>
-    </row>
-    <row r="56" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R55" s="5"/>
+      <c r="S55" s="6"/>
+    </row>
+    <row r="56" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="14"/>
       <c r="B56" s="7"/>
       <c r="C56" s="17"/>
@@ -1930,8 +2040,10 @@
       <c r="O56" s="9"/>
       <c r="P56" s="8"/>
       <c r="Q56" s="9"/>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R56" s="8"/>
+      <c r="S56" s="9"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="13"/>
       <c r="B57" s="4"/>
       <c r="C57" s="16"/>
@@ -1949,8 +2061,10 @@
       <c r="O57" s="6"/>
       <c r="P57" s="5"/>
       <c r="Q57" s="6"/>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R57" s="5"/>
+      <c r="S57" s="6"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="13"/>
       <c r="B58" s="4"/>
       <c r="C58" s="16"/>
@@ -1968,8 +2082,10 @@
       <c r="O58" s="6"/>
       <c r="P58" s="5"/>
       <c r="Q58" s="6"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R58" s="5"/>
+      <c r="S58" s="6"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="13"/>
       <c r="B59" s="4"/>
       <c r="C59" s="16"/>
@@ -1987,8 +2103,10 @@
       <c r="O59" s="6"/>
       <c r="P59" s="5"/>
       <c r="Q59" s="6"/>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R59" s="5"/>
+      <c r="S59" s="6"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="13"/>
       <c r="B60" s="4"/>
       <c r="C60" s="16"/>
@@ -2006,8 +2124,10 @@
       <c r="O60" s="6"/>
       <c r="P60" s="5"/>
       <c r="Q60" s="6"/>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R60" s="5"/>
+      <c r="S60" s="6"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="13"/>
       <c r="B61" s="4"/>
       <c r="C61" s="16"/>
@@ -2025,8 +2145,10 @@
       <c r="O61" s="6"/>
       <c r="P61" s="5"/>
       <c r="Q61" s="6"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R61" s="5"/>
+      <c r="S61" s="6"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="13"/>
       <c r="B62" s="4"/>
       <c r="C62" s="16"/>
@@ -2044,8 +2166,10 @@
       <c r="O62" s="6"/>
       <c r="P62" s="5"/>
       <c r="Q62" s="6"/>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R62" s="5"/>
+      <c r="S62" s="6"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="13"/>
       <c r="B63" s="4"/>
       <c r="C63" s="16"/>
@@ -2063,8 +2187,10 @@
       <c r="O63" s="6"/>
       <c r="P63" s="5"/>
       <c r="Q63" s="6"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R63" s="5"/>
+      <c r="S63" s="6"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="13"/>
       <c r="B64" s="4"/>
       <c r="C64" s="16"/>
@@ -2082,8 +2208,10 @@
       <c r="O64" s="6"/>
       <c r="P64" s="5"/>
       <c r="Q64" s="6"/>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R64" s="5"/>
+      <c r="S64" s="6"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="13"/>
       <c r="B65" s="4"/>
       <c r="C65" s="16"/>
@@ -2101,8 +2229,10 @@
       <c r="O65" s="6"/>
       <c r="P65" s="5"/>
       <c r="Q65" s="6"/>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R65" s="5"/>
+      <c r="S65" s="6"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" s="13"/>
       <c r="B66" s="4"/>
       <c r="C66" s="16"/>
@@ -2120,8 +2250,10 @@
       <c r="O66" s="6"/>
       <c r="P66" s="5"/>
       <c r="Q66" s="6"/>
-    </row>
-    <row r="67" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R66" s="5"/>
+      <c r="S66" s="6"/>
+    </row>
+    <row r="67" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="14"/>
       <c r="B67" s="7"/>
       <c r="C67" s="17"/>
@@ -2139,28 +2271,32 @@
       <c r="O67" s="9"/>
       <c r="P67" s="8"/>
       <c r="Q67" s="9"/>
+      <c r="R67" s="8"/>
+      <c r="S67" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="P2:Q3"/>
-    <mergeCell ref="B2:M3"/>
+  <mergeCells count="21">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="B2:M3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q5"/>
+    <mergeCell ref="R4:S5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="N5:O5"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P2:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>